<commit_message>
wrote some code in some text files, also made some graphs in some notebook
</commit_message>
<xml_diff>
--- a/Cleaned JSON and XLSX/surveydata.xlsx
+++ b/Cleaned JSON and XLSX/surveydata.xlsx
@@ -1479,7 +1479,7 @@
         <v>4</v>
       </c>
       <c r="W2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="X2">
         <v>2</v>
@@ -1631,7 +1631,7 @@
         <v>2</v>
       </c>
       <c r="W3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X3">
         <v>2</v>
@@ -1777,7 +1777,7 @@
         <v>3</v>
       </c>
       <c r="W4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -1926,7 +1926,7 @@
         <v>3</v>
       </c>
       <c r="W5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X5">
         <v>2</v>
@@ -2078,7 +2078,7 @@
         <v>2</v>
       </c>
       <c r="W6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -2224,7 +2224,7 @@
         <v>3</v>
       </c>
       <c r="W7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X7">
         <v>1</v>
@@ -2370,7 +2370,7 @@
         <v>4</v>
       </c>
       <c r="W8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X8">
         <v>1</v>
@@ -2525,7 +2525,7 @@
         <v>3</v>
       </c>
       <c r="W9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X9">
         <v>1</v>
@@ -2677,7 +2677,7 @@
         <v>5</v>
       </c>
       <c r="W10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X10">
         <v>3</v>
@@ -2823,7 +2823,7 @@
         <v>4</v>
       </c>
       <c r="W11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X11">
         <v>4</v>
@@ -2969,7 +2969,7 @@
         <v>3</v>
       </c>
       <c r="W12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X12">
         <v>2</v>
@@ -3115,7 +3115,7 @@
         <v>3</v>
       </c>
       <c r="W13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X13">
         <v>1</v>
@@ -3258,7 +3258,7 @@
         <v>3</v>
       </c>
       <c r="W14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X14">
         <v>5</v>
@@ -3404,7 +3404,7 @@
         <v>3</v>
       </c>
       <c r="W15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X15">
         <v>2</v>
@@ -3553,7 +3553,7 @@
         <v>2</v>
       </c>
       <c r="W16">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X16">
         <v>1</v>
@@ -3696,7 +3696,7 @@
         <v>1</v>
       </c>
       <c r="W17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X17">
         <v>3</v>
@@ -3845,7 +3845,7 @@
         <v>4</v>
       </c>
       <c r="W18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="X18">
         <v>4</v>
@@ -3994,7 +3994,7 @@
         <v>2</v>
       </c>
       <c r="W19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="X19">
         <v>4</v>
@@ -4140,7 +4140,7 @@
         <v>3</v>
       </c>
       <c r="W20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X20">
         <v>3</v>
@@ -4286,7 +4286,7 @@
         <v>1</v>
       </c>
       <c r="W21">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X21">
         <v>1</v>
@@ -4435,7 +4435,7 @@
         <v>4</v>
       </c>
       <c r="W22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X22">
         <v>1</v>
@@ -4584,7 +4584,7 @@
         <v>4</v>
       </c>
       <c r="W23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="X23">
         <v>3</v>
@@ -4882,7 +4882,7 @@
         <v>2</v>
       </c>
       <c r="W25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X25">
         <v>3</v>
@@ -5028,7 +5028,7 @@
         <v>4</v>
       </c>
       <c r="W26">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="X26">
         <v>4</v>
@@ -5174,7 +5174,7 @@
         <v>4</v>
       </c>
       <c r="W27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X27">
         <v>4</v>
@@ -5311,7 +5311,7 @@
         <v>5</v>
       </c>
       <c r="W28">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X28">
         <v>3</v>
@@ -5451,7 +5451,7 @@
         <v>4</v>
       </c>
       <c r="W29">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X29">
         <v>1</v>
@@ -5606,7 +5606,7 @@
         <v>4</v>
       </c>
       <c r="W30">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="X30">
         <v>1</v>
@@ -5770,7 +5770,7 @@
         <v>2</v>
       </c>
       <c r="W31">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="X31">
         <v>3</v>
@@ -5931,7 +5931,7 @@
         <v>4</v>
       </c>
       <c r="W32">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="X32">
         <v>4</v>
@@ -6089,7 +6089,7 @@
         <v>2</v>
       </c>
       <c r="W33">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="X33">
         <v>2</v>
@@ -6244,7 +6244,7 @@
         <v>3</v>
       </c>
       <c r="W34">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X34">
         <v>3</v>
@@ -6405,7 +6405,7 @@
         <v>2</v>
       </c>
       <c r="W35">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="X35">
         <v>2</v>
@@ -6557,7 +6557,7 @@
         <v>4</v>
       </c>
       <c r="W36">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="X36">
         <v>1</v>
@@ -6715,7 +6715,7 @@
         <v>3</v>
       </c>
       <c r="W37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X37">
         <v>3</v>
@@ -6873,19 +6873,19 @@
         <v>262</v>
       </c>
       <c r="V38">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W38">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="X38">
         <v>1</v>
       </c>
       <c r="Y38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z38">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AA38" t="s">
         <v>269</v>

</xml_diff>